<commit_message>
fixed a bug from arduino_script.py line 17. The bug works by catching an sqlite3.Error and printing "Something went wrong" but it should not.
</commit_message>
<xml_diff>
--- a/sources/Tayabas/Tayabas-Data.xlsx
+++ b/sources/Tayabas/Tayabas-Data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Data Collected from Tayabas</t>
+  </si>
   <si>
     <t xml:space="preserve">Controlled Group (OpenWeatherMap’s Weather Forecast)</t>
   </si>
@@ -42,6 +45,522 @@
   <si>
     <t xml:space="preserve">Sample Size</t>
   </si>
+  <si>
+    <t xml:space="preserve">Data Collected from Tagkawayan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Controlled Group (OpenWeatherMap’s Weather Forecast)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Experimental Group (Localized Crop Recommendation System)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+Sample Size
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1
+1016.13
+28.19
+100.00%
+1
+995.68300981461
+27.8195748785721
+87.848309807065
+917
+2
+1016.13
+28.19
+100
+2
+995.898391089109
+27.6738859917859
+88.1003713230095
+808
+3
+1016.13
+28.19
+100
+3
+995.942946635731
+27.6381088537852
+87.7331788755625
+860
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Controlled Group (OpenWeatherMap’s Weather Forecast)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Experimental Group (Localized Crop Recommendation System)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+Sample Size
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1
+1016.13
+28.19
+100.00%
+1
+995.68300981461
+27.8195748785721
+87.848309807065
+917
+2
+1016.13
+28.19
+100
+2
+995.898391089109
+27.6738859917859
+88.1003713230095
+808
+3
+1016.13
+28.19
+100
+3
+995.942946635731
+27.6381088537852
+87.7331788755625
+860
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Controlled Group (OpenWeatherMap’s Weather Forecast)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Experimental Group (Localized Crop Recommendation System)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+Sample Size
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1
+1016.13
+28.19
+100.00%
+1
+995.68300981461
+27.8195748785721
+87.848309807065
+917
+2
+1016.13
+28.19
+100
+2
+995.898391089109
+27.6738859917859
+88.1003713230095
+808
+3
+1016.13
+28.19
+100
+3
+995.942946635731
+27.</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Controlled Group (OpenWeatherMap’s Weather Forecast)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Experimental Group (Localized Crop Recommendation System)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Trial
+Pressure (hPa)
+Temperature (*C)
+Humidity (%)
+Sample Size
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1
+1016.13
+28.19
+100.00%
+1
+995.68300981461
+27.8195748785721
+87.848309807065
+917
+2
+1016.13
+28.19
+100
+2
+995.898391089109
+27.6738859917859
+88.1003713230095
+808
+3
+1016.13
+28.19
+100
+3
+995.942946635731
+27.6381088537852
+87.7331788755625
+860
+87.7331788755625
+860
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -51,7 +570,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -78,6 +597,26 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -123,7 +662,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -136,6 +675,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -144,11 +687,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,10 +720,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -190,11 +741,16 @@
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -203,48 +759,48 @@
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,19 +813,19 @@
       <c r="C8" s="1" t="n">
         <v>28.19</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="8" t="n">
         <v>995.68300981461</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>27.8195748785721</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="8" t="n">
         <v>87.848309807065</v>
       </c>
       <c r="J8" s="1" t="n">
@@ -334,10 +890,155 @@
         <v>860</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="3014.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1016.13</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>28.19</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>27.8195748785721</v>
+      </c>
+      <c r="I21" s="8" t="n">
+        <v>87.848309807065</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>1016.13</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>28.19</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>995.898391089109</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>27.6738859917859</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>88.1003713230095</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>1016.13</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>28.19</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>995.942946635731</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>27.6381088537852</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>87.7331788755625</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>860</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="C2:G2"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="F4:J4"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:J17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>